<commit_message>
Stable MBS Version Running Spring and Dampers
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/flyball_governor/flyball_governor_gravity_damper.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/flyball_governor/flyball_governor_gravity_damper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\flyball_governor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B086FB-F942-4ED9-8F12-2B05FC917D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE0A221-CFFB-4F74-981D-155B7F07840B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="253">
   <si>
     <t>Mass</t>
   </si>
@@ -1122,7 +1122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1315,6 +1315,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1969,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B2:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1989,44 +1995,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="82"/>
-      <c r="J2" s="78" t="s">
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="84"/>
+      <c r="J2" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="75"/>
+      <c r="C3" s="77"/>
       <c r="D3" s="52">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E3" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="J3" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="77"/>
+      <c r="K3" s="79"/>
       <c r="L3" s="56"/>
-      <c r="M3" s="76" t="s">
+      <c r="M3" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="N3" s="77"/>
-      <c r="O3" s="83"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="85"/>
       <c r="P3" s="47" t="s">
         <v>163</v>
       </c>
@@ -2035,12 +2041,12 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="75"/>
+      <c r="C4" s="77"/>
       <c r="D4" s="52">
-        <v>3.0000000000000001E-3</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="E4" s="52" t="s">
         <v>22</v>
@@ -2058,7 +2064,7 @@
       <c r="N4" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="O4" s="84"/>
+      <c r="O4" s="86"/>
       <c r="P4" s="47" t="s">
         <v>164</v>
       </c>
@@ -2067,10 +2073,10 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="76" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="75"/>
+      <c r="C5" s="77"/>
       <c r="D5" s="52" t="s">
         <v>84</v>
       </c>
@@ -2090,7 +2096,7 @@
       <c r="N5" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="84"/>
+      <c r="O5" s="86"/>
       <c r="P5" s="47" t="s">
         <v>165</v>
       </c>
@@ -2099,10 +2105,10 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="75"/>
+      <c r="C6" s="77"/>
       <c r="D6" s="52" t="s">
         <v>3</v>
       </c>
@@ -2122,7 +2128,7 @@
       <c r="N6" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="O6" s="84"/>
+      <c r="O6" s="86"/>
       <c r="P6" s="47" t="s">
         <v>169</v>
       </c>
@@ -2131,10 +2137,10 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="75"/>
+      <c r="C7" s="77"/>
       <c r="D7" s="52">
         <v>-9806.65</v>
       </c>
@@ -2154,7 +2160,7 @@
       <c r="N7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="84"/>
+      <c r="O7" s="86"/>
       <c r="P7" s="47" t="s">
         <v>168</v>
       </c>
@@ -2163,10 +2169,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="75"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="52" t="s">
         <v>131</v>
       </c>
@@ -2186,7 +2192,7 @@
       <c r="N8" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="84"/>
+      <c r="O8" s="86"/>
       <c r="P8" s="47" t="s">
         <v>172</v>
       </c>
@@ -2195,10 +2201,10 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="75"/>
+      <c r="C9" s="77"/>
       <c r="D9" s="52"/>
       <c r="E9" s="53" t="s">
         <v>125</v>
@@ -2216,7 +2222,7 @@
       <c r="N9" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="O9" s="84"/>
+      <c r="O9" s="86"/>
       <c r="P9" s="47" t="s">
         <v>173</v>
       </c>
@@ -2238,7 +2244,7 @@
       <c r="N10" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="84"/>
+      <c r="O10" s="86"/>
       <c r="P10" s="51" t="s">
         <v>174</v>
       </c>
@@ -2256,7 +2262,7 @@
       <c r="N11" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="O11" s="84"/>
+      <c r="O11" s="86"/>
       <c r="P11" s="51" t="s">
         <v>175</v>
       </c>
@@ -2265,15 +2271,15 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="80" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
       <c r="J12" s="57"/>
       <c r="K12" s="58"/>
       <c r="L12" s="58"/>
@@ -2283,7 +2289,7 @@
       <c r="N12" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="O12" s="84"/>
+      <c r="O12" s="86"/>
       <c r="P12" s="47" t="s">
         <v>180</v>
       </c>
@@ -2292,17 +2298,19 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="C13" s="79"/>
-      <c r="D13" s="70"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="70" t="s">
+        <v>241</v>
+      </c>
       <c r="E13" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
       <c r="J13" s="57"/>
       <c r="K13" s="58"/>
       <c r="L13" s="58"/>
@@ -2312,7 +2320,7 @@
       <c r="N13" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="84"/>
+      <c r="O13" s="86"/>
       <c r="P13" s="51" t="s">
         <v>181</v>
       </c>
@@ -2321,17 +2329,19 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="79"/>
-      <c r="D14" s="70"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="70" t="s">
+        <v>241</v>
+      </c>
       <c r="E14" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="F14" s="109"/>
-      <c r="G14" s="109"/>
-      <c r="H14" s="109"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
       <c r="J14" s="59"/>
       <c r="K14" s="60"/>
       <c r="L14" s="58"/>
@@ -2341,7 +2351,7 @@
       <c r="N14" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="O14" s="84"/>
+      <c r="O14" s="86"/>
       <c r="P14" s="51" t="s">
         <v>182</v>
       </c>
@@ -2350,21 +2360,21 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="79"/>
+      <c r="C15" s="81"/>
       <c r="D15" s="70"/>
       <c r="E15" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="J15" s="76" t="s">
+      <c r="F15" s="111"/>
+      <c r="G15" s="111"/>
+      <c r="H15" s="111"/>
+      <c r="J15" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="K15" s="77"/>
+      <c r="K15" s="79"/>
       <c r="L15" s="58"/>
       <c r="M15" s="47" t="s">
         <v>15</v>
@@ -2372,7 +2382,7 @@
       <c r="N15" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="84"/>
+      <c r="O15" s="86"/>
       <c r="P15" s="51" t="s">
         <v>183</v>
       </c>
@@ -2381,17 +2391,19 @@
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="79" t="s">
+      <c r="B16" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="C16" s="79"/>
-      <c r="D16" s="70"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="70" t="s">
+        <v>241</v>
+      </c>
       <c r="E16" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="F16" s="109"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="109"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="111"/>
+      <c r="H16" s="111"/>
       <c r="J16" s="47" t="s">
         <v>96</v>
       </c>
@@ -2405,7 +2417,7 @@
       <c r="N16" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="O16" s="84"/>
+      <c r="O16" s="86"/>
       <c r="P16" s="47" t="s">
         <v>188</v>
       </c>
@@ -2414,17 +2426,17 @@
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="79"/>
+      <c r="C17" s="81"/>
       <c r="D17" s="70"/>
       <c r="E17" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="109"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="111"/>
       <c r="J17" s="47" t="s">
         <v>0</v>
       </c>
@@ -2432,11 +2444,11 @@
         <v>101</v>
       </c>
       <c r="L17" s="58"/>
-      <c r="M17" s="76" t="s">
+      <c r="M17" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="N17" s="77"/>
-      <c r="O17" s="84"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="86"/>
       <c r="P17" s="51" t="s">
         <v>189</v>
       </c>
@@ -2445,17 +2457,19 @@
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="85" t="s">
+      <c r="B18" s="87" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="86"/>
-      <c r="D18" s="46"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="46" t="s">
+        <v>241</v>
+      </c>
       <c r="E18" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="F18" s="109"/>
-      <c r="G18" s="109"/>
-      <c r="H18" s="109"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="111"/>
       <c r="J18" s="47" t="s">
         <v>97</v>
       </c>
@@ -2469,7 +2483,7 @@
       <c r="N18" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="O18" s="84"/>
+      <c r="O18" s="86"/>
       <c r="P18" s="51" t="s">
         <v>190</v>
       </c>
@@ -2478,17 +2492,17 @@
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="85" t="s">
+      <c r="B19" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="86"/>
+      <c r="C19" s="88"/>
       <c r="D19" s="46"/>
       <c r="E19" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="F19" s="109"/>
-      <c r="G19" s="109"/>
-      <c r="H19" s="109"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="111"/>
       <c r="J19" s="47" t="s">
         <v>98</v>
       </c>
@@ -2502,7 +2516,7 @@
       <c r="N19" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="O19" s="84"/>
+      <c r="O19" s="86"/>
       <c r="P19" s="51" t="s">
         <v>191</v>
       </c>
@@ -2511,19 +2525,19 @@
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="107" t="s">
+      <c r="B20" s="109" t="s">
         <v>251</v>
       </c>
-      <c r="C20" s="108"/>
+      <c r="C20" s="110"/>
       <c r="D20" s="50" t="s">
         <v>241</v>
       </c>
       <c r="E20" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="F20" s="109"/>
-      <c r="G20" s="109"/>
-      <c r="H20" s="109"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="111"/>
       <c r="J20" s="47" t="s">
         <v>104</v>
       </c>
@@ -2537,7 +2551,7 @@
       <c r="N20" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="O20" s="84"/>
+      <c r="O20" s="86"/>
       <c r="P20" s="47" t="s">
         <v>196</v>
       </c>
@@ -2546,17 +2560,17 @@
       </c>
     </row>
     <row r="21" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="79" t="s">
+      <c r="B21" s="81" t="s">
         <v>252</v>
       </c>
-      <c r="C21" s="79"/>
+      <c r="C21" s="81"/>
       <c r="D21" s="71"/>
       <c r="E21" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="F21" s="109"/>
-      <c r="G21" s="109"/>
-      <c r="H21" s="109"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="111"/>
       <c r="J21" s="47" t="s">
         <v>99</v>
       </c>
@@ -2570,7 +2584,7 @@
       <c r="N21" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="O21" s="84"/>
+      <c r="O21" s="86"/>
       <c r="P21" s="51" t="s">
         <v>197</v>
       </c>
@@ -2579,21 +2593,21 @@
       </c>
     </row>
     <row r="22" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="101" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="100"/>
+      <c r="C22" s="102"/>
       <c r="D22" s="44">
         <v>2</v>
       </c>
-      <c r="E22" s="96" t="s">
+      <c r="E22" s="98" t="s">
         <v>149</v>
       </c>
-      <c r="F22" s="87" t="s">
+      <c r="F22" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="G22" s="88"/>
-      <c r="H22" s="89"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="91"/>
       <c r="J22" s="32" t="s">
         <v>110</v>
       </c>
@@ -2607,7 +2621,7 @@
       <c r="N22" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="O22" s="84"/>
+      <c r="O22" s="86"/>
       <c r="P22" s="51" t="s">
         <v>198</v>
       </c>
@@ -2616,21 +2630,19 @@
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="101"/>
-      <c r="C23" s="102"/>
-      <c r="D23" s="44">
-        <v>3</v>
-      </c>
-      <c r="E23" s="97"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="92"/>
-      <c r="J23" s="105"/>
-      <c r="K23" s="105"/>
-      <c r="L23" s="105"/>
-      <c r="M23" s="105"/>
-      <c r="N23" s="106"/>
-      <c r="O23" s="84"/>
+      <c r="B23" s="103"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="93"/>
+      <c r="H23" s="94"/>
+      <c r="J23" s="107"/>
+      <c r="K23" s="107"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="107"/>
+      <c r="N23" s="108"/>
+      <c r="O23" s="86"/>
       <c r="P23" s="51" t="s">
         <v>199</v>
       </c>
@@ -2639,19 +2651,19 @@
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="101"/>
-      <c r="C24" s="102"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="104"/>
       <c r="D24" s="44"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="91"/>
-      <c r="H24" s="92"/>
-      <c r="J24" s="105"/>
-      <c r="K24" s="105"/>
-      <c r="L24" s="105"/>
-      <c r="M24" s="105"/>
-      <c r="N24" s="106"/>
-      <c r="O24" s="84"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="93"/>
+      <c r="H24" s="94"/>
+      <c r="J24" s="107"/>
+      <c r="K24" s="107"/>
+      <c r="L24" s="107"/>
+      <c r="M24" s="107"/>
+      <c r="N24" s="108"/>
+      <c r="O24" s="86"/>
       <c r="P24" s="32" t="s">
         <v>205</v>
       </c>
@@ -2660,19 +2672,19 @@
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="101"/>
-      <c r="C25" s="102"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="104"/>
       <c r="D25" s="44"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="92"/>
-      <c r="J25" s="105"/>
-      <c r="K25" s="105"/>
-      <c r="L25" s="105"/>
-      <c r="M25" s="105"/>
-      <c r="N25" s="106"/>
-      <c r="O25" s="84"/>
+      <c r="E25" s="99"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="93"/>
+      <c r="H25" s="94"/>
+      <c r="J25" s="107"/>
+      <c r="K25" s="107"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="107"/>
+      <c r="N25" s="108"/>
+      <c r="O25" s="86"/>
       <c r="P25" s="32" t="s">
         <v>209</v>
       </c>
@@ -2681,19 +2693,19 @@
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="101"/>
-      <c r="C26" s="102"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="104"/>
       <c r="D26" s="44"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="92"/>
-      <c r="J26" s="105"/>
-      <c r="K26" s="105"/>
-      <c r="L26" s="105"/>
-      <c r="M26" s="105"/>
-      <c r="N26" s="106"/>
-      <c r="O26" s="84"/>
+      <c r="E26" s="99"/>
+      <c r="F26" s="92"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="94"/>
+      <c r="J26" s="107"/>
+      <c r="K26" s="107"/>
+      <c r="L26" s="107"/>
+      <c r="M26" s="107"/>
+      <c r="N26" s="108"/>
+      <c r="O26" s="86"/>
       <c r="P26" s="32" t="s">
         <v>210</v>
       </c>
@@ -2702,19 +2714,19 @@
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="101"/>
-      <c r="C27" s="102"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="104"/>
       <c r="D27" s="44"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="91"/>
-      <c r="H27" s="92"/>
-      <c r="J27" s="105"/>
-      <c r="K27" s="105"/>
-      <c r="L27" s="105"/>
-      <c r="M27" s="105"/>
-      <c r="N27" s="106"/>
-      <c r="O27" s="84"/>
+      <c r="E27" s="99"/>
+      <c r="F27" s="92"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="94"/>
+      <c r="J27" s="107"/>
+      <c r="K27" s="107"/>
+      <c r="L27" s="107"/>
+      <c r="M27" s="107"/>
+      <c r="N27" s="108"/>
+      <c r="O27" s="86"/>
       <c r="P27" s="32" t="s">
         <v>211</v>
       </c>
@@ -2723,19 +2735,19 @@
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="101"/>
-      <c r="C28" s="102"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="104"/>
       <c r="D28" s="44"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="92"/>
-      <c r="J28" s="105"/>
-      <c r="K28" s="105"/>
-      <c r="L28" s="105"/>
-      <c r="M28" s="105"/>
-      <c r="N28" s="106"/>
-      <c r="O28" s="84"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="94"/>
+      <c r="J28" s="107"/>
+      <c r="K28" s="107"/>
+      <c r="L28" s="107"/>
+      <c r="M28" s="107"/>
+      <c r="N28" s="108"/>
+      <c r="O28" s="86"/>
       <c r="P28" s="32" t="s">
         <v>213</v>
       </c>
@@ -2744,19 +2756,19 @@
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="103"/>
-      <c r="C29" s="104"/>
+      <c r="B29" s="105"/>
+      <c r="C29" s="106"/>
       <c r="D29" s="44"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="93"/>
-      <c r="G29" s="94"/>
-      <c r="H29" s="95"/>
-      <c r="J29" s="105"/>
-      <c r="K29" s="105"/>
-      <c r="L29" s="105"/>
-      <c r="M29" s="105"/>
-      <c r="N29" s="106"/>
-      <c r="O29" s="84"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="96"/>
+      <c r="H29" s="97"/>
+      <c r="J29" s="107"/>
+      <c r="K29" s="107"/>
+      <c r="L29" s="107"/>
+      <c r="M29" s="107"/>
+      <c r="N29" s="108"/>
+      <c r="O29" s="86"/>
       <c r="P29" s="32" t="s">
         <v>212</v>
       </c>
@@ -2765,12 +2777,12 @@
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J30" s="105"/>
-      <c r="K30" s="105"/>
-      <c r="L30" s="105"/>
-      <c r="M30" s="105"/>
-      <c r="N30" s="106"/>
-      <c r="O30" s="84"/>
+      <c r="J30" s="107"/>
+      <c r="K30" s="107"/>
+      <c r="L30" s="107"/>
+      <c r="M30" s="107"/>
+      <c r="N30" s="108"/>
+      <c r="O30" s="86"/>
       <c r="P30" s="32" t="s">
         <v>214</v>
       </c>
@@ -2779,12 +2791,12 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J31" s="105"/>
-      <c r="K31" s="105"/>
-      <c r="L31" s="105"/>
-      <c r="M31" s="105"/>
-      <c r="N31" s="106"/>
-      <c r="O31" s="84"/>
+      <c r="J31" s="107"/>
+      <c r="K31" s="107"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="107"/>
+      <c r="N31" s="108"/>
+      <c r="O31" s="86"/>
       <c r="P31" s="32" t="s">
         <v>215</v>
       </c>
@@ -2793,12 +2805,12 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J32" s="105"/>
-      <c r="K32" s="105"/>
-      <c r="L32" s="105"/>
-      <c r="M32" s="105"/>
-      <c r="N32" s="106"/>
-      <c r="O32" s="84"/>
+      <c r="J32" s="107"/>
+      <c r="K32" s="107"/>
+      <c r="L32" s="107"/>
+      <c r="M32" s="107"/>
+      <c r="N32" s="108"/>
+      <c r="O32" s="86"/>
       <c r="P32" s="32" t="s">
         <v>216</v>
       </c>
@@ -2807,12 +2819,12 @@
       </c>
     </row>
     <row r="33" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J33" s="105"/>
-      <c r="K33" s="105"/>
-      <c r="L33" s="105"/>
-      <c r="M33" s="105"/>
-      <c r="N33" s="106"/>
-      <c r="O33" s="84"/>
+      <c r="J33" s="107"/>
+      <c r="K33" s="107"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="107"/>
+      <c r="N33" s="108"/>
+      <c r="O33" s="86"/>
       <c r="P33" s="32" t="s">
         <v>217</v>
       </c>
@@ -2821,12 +2833,12 @@
       </c>
     </row>
     <row r="34" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J34" s="105"/>
-      <c r="K34" s="105"/>
-      <c r="L34" s="105"/>
-      <c r="M34" s="105"/>
-      <c r="N34" s="106"/>
-      <c r="O34" s="84"/>
+      <c r="J34" s="107"/>
+      <c r="K34" s="107"/>
+      <c r="L34" s="107"/>
+      <c r="M34" s="107"/>
+      <c r="N34" s="108"/>
+      <c r="O34" s="86"/>
       <c r="P34" s="32" t="s">
         <v>218</v>
       </c>
@@ -2835,12 +2847,12 @@
       </c>
     </row>
     <row r="35" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J35" s="105"/>
-      <c r="K35" s="105"/>
-      <c r="L35" s="105"/>
-      <c r="M35" s="105"/>
-      <c r="N35" s="106"/>
-      <c r="O35" s="84"/>
+      <c r="J35" s="107"/>
+      <c r="K35" s="107"/>
+      <c r="L35" s="107"/>
+      <c r="M35" s="107"/>
+      <c r="N35" s="108"/>
+      <c r="O35" s="86"/>
       <c r="P35" s="32" t="s">
         <v>219</v>
       </c>
@@ -2849,12 +2861,12 @@
       </c>
     </row>
     <row r="36" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J36" s="105"/>
-      <c r="K36" s="105"/>
-      <c r="L36" s="105"/>
-      <c r="M36" s="105"/>
-      <c r="N36" s="106"/>
-      <c r="O36" s="84"/>
+      <c r="J36" s="107"/>
+      <c r="K36" s="107"/>
+      <c r="L36" s="107"/>
+      <c r="M36" s="107"/>
+      <c r="N36" s="108"/>
+      <c r="O36" s="86"/>
       <c r="P36" s="32" t="s">
         <v>228</v>
       </c>
@@ -2863,12 +2875,12 @@
       </c>
     </row>
     <row r="37" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J37" s="105"/>
-      <c r="K37" s="105"/>
-      <c r="L37" s="105"/>
-      <c r="M37" s="105"/>
-      <c r="N37" s="106"/>
-      <c r="O37" s="84"/>
+      <c r="J37" s="107"/>
+      <c r="K37" s="107"/>
+      <c r="L37" s="107"/>
+      <c r="M37" s="107"/>
+      <c r="N37" s="108"/>
+      <c r="O37" s="86"/>
       <c r="P37" s="32" t="s">
         <v>229</v>
       </c>
@@ -2877,12 +2889,12 @@
       </c>
     </row>
     <row r="38" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J38" s="105"/>
-      <c r="K38" s="105"/>
-      <c r="L38" s="105"/>
-      <c r="M38" s="105"/>
-      <c r="N38" s="106"/>
-      <c r="O38" s="84"/>
+      <c r="J38" s="107"/>
+      <c r="K38" s="107"/>
+      <c r="L38" s="107"/>
+      <c r="M38" s="107"/>
+      <c r="N38" s="108"/>
+      <c r="O38" s="86"/>
       <c r="P38" s="32" t="s">
         <v>230</v>
       </c>
@@ -2891,12 +2903,12 @@
       </c>
     </row>
     <row r="39" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J39" s="105"/>
-      <c r="K39" s="105"/>
-      <c r="L39" s="105"/>
-      <c r="M39" s="105"/>
-      <c r="N39" s="106"/>
-      <c r="O39" s="84"/>
+      <c r="J39" s="107"/>
+      <c r="K39" s="107"/>
+      <c r="L39" s="107"/>
+      <c r="M39" s="107"/>
+      <c r="N39" s="108"/>
+      <c r="O39" s="86"/>
       <c r="P39" s="32" t="s">
         <v>231</v>
       </c>
@@ -2946,8 +2958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,118 +2978,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="109"/>
-      <c r="B1" s="109"/>
-      <c r="C1" s="79" t="s">
+      <c r="A1" s="111"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79" t="s">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79" t="s">
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79" t="s">
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79" t="s">
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="79"/>
-      <c r="AB1" s="79"/>
-      <c r="AC1" s="79"/>
-      <c r="AD1" s="79"/>
-      <c r="AE1" s="79"/>
-      <c r="AF1" s="79"/>
-      <c r="AG1" s="79"/>
-      <c r="AH1" s="79"/>
-      <c r="AI1" s="79"/>
-      <c r="AJ1" s="79"/>
-      <c r="AK1" s="79"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81"/>
+      <c r="X1" s="81"/>
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
+      <c r="AE1" s="81"/>
+      <c r="AF1" s="81"/>
+      <c r="AG1" s="81"/>
+      <c r="AH1" s="81"/>
+      <c r="AI1" s="81"/>
+      <c r="AJ1" s="81"/>
+      <c r="AK1" s="81"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="109"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="111" t="s">
+      <c r="A2" s="111"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111" t="s">
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111" t="s">
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="79" t="s">
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79" t="s">
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="112" t="s">
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="114" t="s">
         <v>86</v>
       </c>
-      <c r="S2" s="110" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="111" t="s">
+      <c r="S2" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="113" t="s">
         <v>94</v>
       </c>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="79" t="s">
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="85" t="s">
+      <c r="X2" s="81"/>
+      <c r="Y2" s="81"/>
+      <c r="Z2" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="AA2" s="113"/>
-      <c r="AB2" s="86"/>
-      <c r="AC2" s="79" t="s">
+      <c r="AA2" s="115"/>
+      <c r="AB2" s="88"/>
+      <c r="AC2" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="AD2" s="79"/>
-      <c r="AE2" s="79"/>
-      <c r="AF2" s="79" t="s">
+      <c r="AD2" s="81"/>
+      <c r="AE2" s="81"/>
+      <c r="AF2" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="AG2" s="79"/>
-      <c r="AH2" s="79"/>
-      <c r="AI2" s="79" t="s">
+      <c r="AG2" s="81"/>
+      <c r="AH2" s="81"/>
+      <c r="AI2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="AJ2" s="79"/>
-      <c r="AK2" s="79"/>
+      <c r="AJ2" s="81"/>
+      <c r="AK2" s="81"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -3131,8 +3143,8 @@
       <c r="Q3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="112"/>
-      <c r="S3" s="110"/>
+      <c r="R3" s="114"/>
+      <c r="S3" s="112"/>
       <c r="T3" s="16" t="s">
         <v>62</v>
       </c>
@@ -6847,7 +6859,7 @@
   <dimension ref="A1:X65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6867,16 +6879,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -6907,11 +6919,11 @@
       <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -6967,19 +6979,19 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="114" t="s">
+      <c r="A5" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="114"/>
-      <c r="C5" s="114"/>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -7004,16 +7016,16 @@
       <c r="E6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="117" t="s">
+      <c r="F6" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="118"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="117" t="s">
+      <c r="G6" s="120"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="118"/>
-      <c r="K6" s="119"/>
+      <c r="J6" s="120"/>
+      <c r="K6" s="121"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="20"/>
@@ -7049,22 +7061,22 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="114" t="s">
+      <c r="A8" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="114"/>
-      <c r="H8" s="114"/>
-      <c r="I8" s="114"/>
-      <c r="J8" s="114"/>
-      <c r="K8" s="114"/>
-      <c r="L8" s="114"/>
-      <c r="M8" s="114"/>
-      <c r="N8" s="114"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="116"/>
+      <c r="K8" s="116"/>
+      <c r="L8" s="116"/>
+      <c r="M8" s="116"/>
+      <c r="N8" s="116"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -7089,21 +7101,21 @@
       <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="115" t="s">
+      <c r="F9" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="115"/>
-      <c r="H9" s="115"/>
-      <c r="I9" s="116" t="s">
+      <c r="G9" s="117"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="116"/>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116" t="s">
+      <c r="J9" s="118"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="M9" s="116"/>
-      <c r="N9" s="116"/>
+      <c r="M9" s="118"/>
+      <c r="N9" s="118"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -7157,19 +7169,19 @@
       <c r="X11" s="10"/>
     </row>
     <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="114"/>
-      <c r="I12" s="114"/>
-      <c r="J12" s="114"/>
-      <c r="K12" s="114"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="116"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
@@ -7194,16 +7206,16 @@
       <c r="E13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="115" t="s">
+      <c r="F13" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="115"/>
-      <c r="H13" s="115"/>
-      <c r="I13" s="116" t="s">
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="116"/>
-      <c r="K13" s="116"/>
+      <c r="J13" s="118"/>
+      <c r="K13" s="118"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -7345,19 +7357,19 @@
       <c r="X17" s="10"/>
     </row>
     <row r="18" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="114" t="s">
+      <c r="A18" s="116" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="114"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="114"/>
-      <c r="J18" s="114"/>
-      <c r="K18" s="114"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
+      <c r="G18" s="116"/>
+      <c r="H18" s="116"/>
+      <c r="I18" s="116"/>
+      <c r="J18" s="116"/>
+      <c r="K18" s="116"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
@@ -7382,16 +7394,16 @@
       <c r="E19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="115" t="s">
+      <c r="F19" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="115"/>
-      <c r="H19" s="115"/>
-      <c r="I19" s="116" t="s">
+      <c r="G19" s="117"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="116"/>
-      <c r="K19" s="116"/>
+      <c r="J19" s="118"/>
+      <c r="K19" s="118"/>
     </row>
     <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -7428,19 +7440,19 @@
       <c r="X21" s="10"/>
     </row>
     <row r="22" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="114" t="s">
+      <c r="A22" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="114"/>
-      <c r="C22" s="114"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="114"/>
-      <c r="F22" s="114"/>
-      <c r="G22" s="114"/>
-      <c r="H22" s="114"/>
-      <c r="I22" s="114"/>
-      <c r="J22" s="114"/>
-      <c r="K22" s="114"/>
+      <c r="B22" s="116"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="116"/>
+      <c r="G22" s="116"/>
+      <c r="H22" s="116"/>
+      <c r="I22" s="116"/>
+      <c r="J22" s="116"/>
+      <c r="K22" s="116"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
@@ -7465,16 +7477,16 @@
       <c r="E23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="115" t="s">
+      <c r="F23" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="115"/>
-      <c r="H23" s="115"/>
-      <c r="I23" s="116" t="s">
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="116"/>
-      <c r="K23" s="116"/>
+      <c r="J23" s="118"/>
+      <c r="K23" s="118"/>
     </row>
     <row r="24" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
@@ -7511,22 +7523,22 @@
     </row>
     <row r="25" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="114" t="s">
+      <c r="A26" s="116" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="114"/>
-      <c r="C26" s="114"/>
-      <c r="D26" s="114"/>
-      <c r="E26" s="114"/>
-      <c r="F26" s="114"/>
-      <c r="G26" s="114"/>
-      <c r="H26" s="114"/>
-      <c r="I26" s="114"/>
-      <c r="J26" s="114"/>
-      <c r="K26" s="114"/>
-      <c r="L26" s="114"/>
-      <c r="M26" s="114"/>
-      <c r="N26" s="114"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="116"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="116"/>
+      <c r="G26" s="116"/>
+      <c r="H26" s="116"/>
+      <c r="I26" s="116"/>
+      <c r="J26" s="116"/>
+      <c r="K26" s="116"/>
+      <c r="L26" s="116"/>
+      <c r="M26" s="116"/>
+      <c r="N26" s="116"/>
     </row>
     <row r="27" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
@@ -7544,44 +7556,44 @@
       <c r="E27" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="115" t="s">
+      <c r="F27" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="G27" s="115"/>
-      <c r="H27" s="115"/>
-      <c r="I27" s="116" t="s">
+      <c r="G27" s="117"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="118" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="116"/>
-      <c r="K27" s="116"/>
-      <c r="L27" s="116" t="s">
+      <c r="J27" s="118"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="M27" s="116"/>
-      <c r="N27" s="116"/>
+      <c r="M27" s="118"/>
+      <c r="N27" s="118"/>
     </row>
     <row r="28" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="114" t="s">
+      <c r="A30" s="116" t="s">
         <v>128</v>
       </c>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="114"/>
-      <c r="I30" s="114"/>
-      <c r="J30" s="114"/>
-      <c r="K30" s="114"/>
-      <c r="L30" s="114"/>
-      <c r="M30" s="114"/>
-      <c r="N30" s="114"/>
-      <c r="O30" s="114"/>
-      <c r="P30" s="114"/>
-      <c r="Q30" s="114"/>
+      <c r="B30" s="116"/>
+      <c r="C30" s="116"/>
+      <c r="D30" s="116"/>
+      <c r="E30" s="116"/>
+      <c r="F30" s="116"/>
+      <c r="G30" s="116"/>
+      <c r="H30" s="116"/>
+      <c r="I30" s="116"/>
+      <c r="J30" s="116"/>
+      <c r="K30" s="116"/>
+      <c r="L30" s="116"/>
+      <c r="M30" s="116"/>
+      <c r="N30" s="116"/>
+      <c r="O30" s="116"/>
+      <c r="P30" s="116"/>
+      <c r="Q30" s="116"/>
     </row>
     <row r="31" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
@@ -7599,26 +7611,26 @@
       <c r="E31" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="117" t="s">
+      <c r="F31" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="118"/>
-      <c r="H31" s="119"/>
-      <c r="I31" s="117" t="s">
+      <c r="G31" s="120"/>
+      <c r="H31" s="121"/>
+      <c r="I31" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="118"/>
-      <c r="K31" s="119"/>
-      <c r="L31" s="116" t="s">
+      <c r="J31" s="120"/>
+      <c r="K31" s="121"/>
+      <c r="L31" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="M31" s="116"/>
-      <c r="N31" s="116"/>
-      <c r="O31" s="116" t="s">
+      <c r="M31" s="118"/>
+      <c r="N31" s="118"/>
+      <c r="O31" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="P31" s="116"/>
-      <c r="Q31" s="116"/>
+      <c r="P31" s="118"/>
+      <c r="Q31" s="118"/>
     </row>
     <row r="32" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
@@ -7641,14 +7653,14 @@
     </row>
     <row r="33" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="114" t="s">
+      <c r="A34" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="114"/>
-      <c r="C34" s="114"/>
-      <c r="D34" s="114"/>
-      <c r="E34" s="114"/>
-      <c r="F34" s="114"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="116"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="116"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
@@ -7726,12 +7738,12 @@
       <c r="X37" s="10"/>
     </row>
     <row r="38" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="114" t="s">
+      <c r="A38" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="114"/>
-      <c r="C38" s="114"/>
-      <c r="D38" s="114"/>
+      <c r="B38" s="116"/>
+      <c r="C38" s="116"/>
+      <c r="D38" s="116"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -7824,15 +7836,15 @@
       <c r="Q41" s="10"/>
     </row>
     <row r="42" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="120" t="s">
+      <c r="A42" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="121"/>
-      <c r="C42" s="121"/>
-      <c r="D42" s="121"/>
-      <c r="E42" s="121"/>
-      <c r="F42" s="121"/>
-      <c r="G42" s="122"/>
+      <c r="B42" s="123"/>
+      <c r="C42" s="123"/>
+      <c r="D42" s="123"/>
+      <c r="E42" s="123"/>
+      <c r="F42" s="123"/>
+      <c r="G42" s="124"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -7856,11 +7868,11 @@
       <c r="D43" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="116" t="s">
+      <c r="E43" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="F43" s="116"/>
-      <c r="G43" s="116"/>
+      <c r="F43" s="118"/>
+      <c r="G43" s="118"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8179,7 +8191,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8193,18 +8205,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="128" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -8222,11 +8234,11 @@
       <c r="E2" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="123" t="s">
+      <c r="F2" s="125" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="124"/>
-      <c r="H2" s="125"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="127"/>
       <c r="I2" s="25" t="s">
         <v>49</v>
       </c>
@@ -8255,8 +8267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F55610B-D925-4735-AE3D-EBBD0AD81ACC}">
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22:N23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8279,58 +8291,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="131" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
-      <c r="O1" s="130"/>
-      <c r="P1" s="130"/>
-      <c r="Q1" s="130"/>
-      <c r="R1" s="130"/>
-      <c r="S1" s="130"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="132"/>
+      <c r="L1" s="132"/>
+      <c r="M1" s="132"/>
+      <c r="N1" s="132"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
+      <c r="R1" s="132"/>
+      <c r="S1" s="132"/>
     </row>
     <row r="2" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="114"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="131" t="s">
+      <c r="A2" s="116"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="133" t="s">
         <v>115</v>
       </c>
-      <c r="O2" s="132"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="132"/>
-      <c r="R2" s="132"/>
-      <c r="S2" s="133"/>
-      <c r="V2" s="138" t="s">
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
+      <c r="S2" s="135"/>
+      <c r="V2" s="140" t="s">
         <v>123</v>
       </c>
-      <c r="W2" s="138"/>
-      <c r="X2" s="138"/>
-      <c r="Y2" s="138"/>
-      <c r="Z2" s="138"/>
-      <c r="AA2" s="138"/>
+      <c r="W2" s="140"/>
+      <c r="X2" s="140"/>
+      <c r="Y2" s="140"/>
+      <c r="Z2" s="140"/>
+      <c r="AA2" s="140"/>
     </row>
     <row r="3" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
@@ -8348,16 +8360,16 @@
       <c r="E3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="139" t="s">
+      <c r="F3" s="141" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="140"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="143" t="s">
+      <c r="G3" s="142"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="144"/>
-      <c r="K3" s="145"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="147"/>
       <c r="L3" s="66" t="s">
         <v>249</v>
       </c>
@@ -8376,132 +8388,176 @@
       <c r="Q3" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="R3" s="142" t="s">
+      <c r="R3" s="144" t="s">
         <v>122</v>
       </c>
-      <c r="S3" s="142"/>
-      <c r="V3" s="138"/>
-      <c r="W3" s="138"/>
-      <c r="X3" s="138"/>
-      <c r="Y3" s="138"/>
-      <c r="Z3" s="138"/>
-      <c r="AA3" s="138"/>
+      <c r="S3" s="144"/>
+      <c r="V3" s="140"/>
+      <c r="W3" s="140"/>
+      <c r="X3" s="140"/>
+      <c r="Y3" s="140"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="140"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="18"/>
+      <c r="B4" s="74" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74">
+        <v>2</v>
+      </c>
+      <c r="E4" s="74">
+        <v>4</v>
+      </c>
+      <c r="F4" s="74">
+        <v>-50</v>
+      </c>
+      <c r="G4" s="74">
+        <v>500</v>
+      </c>
+      <c r="H4" s="74">
+        <v>0</v>
+      </c>
+      <c r="I4" s="74">
+        <v>-460</v>
+      </c>
+      <c r="J4" s="74">
+        <v>750</v>
+      </c>
+      <c r="K4" s="74">
+        <v>0</v>
+      </c>
+      <c r="L4" s="74">
+        <v>500</v>
+      </c>
+      <c r="M4" s="18">
+        <v>800</v>
+      </c>
       <c r="N4" s="41"/>
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
-      <c r="V4" s="138"/>
-      <c r="W4" s="138"/>
-      <c r="X4" s="138"/>
-      <c r="Y4" s="138"/>
-      <c r="Z4" s="138"/>
-      <c r="AA4" s="138"/>
+      <c r="V4" s="140"/>
+      <c r="W4" s="140"/>
+      <c r="X4" s="140"/>
+      <c r="Y4" s="140"/>
+      <c r="Z4" s="140"/>
+      <c r="AA4" s="140"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="18"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="74" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74">
+        <v>2</v>
+      </c>
+      <c r="E5" s="74">
+        <v>5</v>
+      </c>
+      <c r="F5" s="74">
+        <v>50</v>
+      </c>
+      <c r="G5" s="74">
+        <v>500</v>
+      </c>
+      <c r="H5" s="74">
+        <v>0</v>
+      </c>
+      <c r="I5" s="74">
+        <v>460</v>
+      </c>
+      <c r="J5" s="74">
+        <v>750</v>
+      </c>
+      <c r="K5" s="74">
+        <v>0</v>
+      </c>
+      <c r="L5" s="74">
+        <v>500</v>
+      </c>
+      <c r="M5" s="18">
+        <v>800</v>
+      </c>
       <c r="N5" s="49"/>
       <c r="O5" s="49"/>
       <c r="P5" s="49"/>
       <c r="Q5" s="49"/>
       <c r="R5" s="49"/>
       <c r="S5" s="49"/>
-      <c r="V5" s="138"/>
-      <c r="W5" s="138"/>
-      <c r="X5" s="138"/>
-      <c r="Y5" s="138"/>
-      <c r="Z5" s="138"/>
-      <c r="AA5" s="138"/>
+      <c r="V5" s="140"/>
+      <c r="W5" s="140"/>
+      <c r="X5" s="140"/>
+      <c r="Y5" s="140"/>
+      <c r="Z5" s="140"/>
+      <c r="AA5" s="140"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V6" s="138"/>
-      <c r="W6" s="138"/>
-      <c r="X6" s="138"/>
-      <c r="Y6" s="138"/>
-      <c r="Z6" s="138"/>
-      <c r="AA6" s="138"/>
+      <c r="V6" s="140"/>
+      <c r="W6" s="140"/>
+      <c r="X6" s="140"/>
+      <c r="Y6" s="140"/>
+      <c r="Z6" s="140"/>
+      <c r="AA6" s="140"/>
     </row>
     <row r="7" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="129" t="s">
+      <c r="A7" s="131" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="130"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="130"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="130"/>
-      <c r="K7" s="130"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="130"/>
-      <c r="N7" s="130"/>
-      <c r="O7" s="130"/>
-      <c r="P7" s="130"/>
-      <c r="Q7" s="130"/>
-      <c r="R7" s="130"/>
-      <c r="V7" s="138"/>
-      <c r="W7" s="138"/>
-      <c r="X7" s="138"/>
-      <c r="Y7" s="138"/>
-      <c r="Z7" s="138"/>
-      <c r="AA7" s="138"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="132"/>
+      <c r="K7" s="132"/>
+      <c r="L7" s="132"/>
+      <c r="M7" s="132"/>
+      <c r="N7" s="132"/>
+      <c r="O7" s="132"/>
+      <c r="P7" s="132"/>
+      <c r="Q7" s="132"/>
+      <c r="R7" s="132"/>
+      <c r="V7" s="140"/>
+      <c r="W7" s="140"/>
+      <c r="X7" s="140"/>
+      <c r="Y7" s="140"/>
+      <c r="Z7" s="140"/>
+      <c r="AA7" s="140"/>
     </row>
     <row r="8" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="114"/>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="114"/>
-      <c r="H8" s="114"/>
-      <c r="I8" s="114"/>
-      <c r="J8" s="114"/>
-      <c r="K8" s="114"/>
-      <c r="L8" s="114"/>
-      <c r="M8" s="114"/>
-      <c r="N8" s="146" t="s">
+      <c r="A8" s="116"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="116"/>
+      <c r="K8" s="116"/>
+      <c r="L8" s="116"/>
+      <c r="M8" s="116"/>
+      <c r="N8" s="148" t="s">
         <v>119</v>
       </c>
-      <c r="O8" s="146"/>
-      <c r="P8" s="146"/>
-      <c r="Q8" s="146"/>
-      <c r="R8" s="146"/>
-      <c r="V8" s="138"/>
-      <c r="W8" s="138"/>
-      <c r="X8" s="138"/>
-      <c r="Y8" s="138"/>
-      <c r="Z8" s="138"/>
-      <c r="AA8" s="138"/>
+      <c r="O8" s="148"/>
+      <c r="P8" s="148"/>
+      <c r="Q8" s="148"/>
+      <c r="R8" s="148"/>
+      <c r="V8" s="140"/>
+      <c r="W8" s="140"/>
+      <c r="X8" s="140"/>
+      <c r="Y8" s="140"/>
+      <c r="Z8" s="140"/>
+      <c r="AA8" s="140"/>
     </row>
     <row r="9" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
@@ -8519,16 +8575,16 @@
       <c r="E9" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="139" t="s">
+      <c r="F9" s="141" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="140"/>
-      <c r="H9" s="141"/>
-      <c r="I9" s="143" t="s">
+      <c r="G9" s="142"/>
+      <c r="H9" s="143"/>
+      <c r="I9" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="144"/>
-      <c r="K9" s="145"/>
+      <c r="J9" s="146"/>
+      <c r="K9" s="147"/>
       <c r="L9" s="40" t="s">
         <v>114</v>
       </c>
@@ -8544,16 +8600,16 @@
       <c r="P9" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="Q9" s="139" t="s">
+      <c r="Q9" s="141" t="s">
         <v>121</v>
       </c>
-      <c r="R9" s="141"/>
-      <c r="V9" s="138"/>
-      <c r="W9" s="138"/>
-      <c r="X9" s="138"/>
-      <c r="Y9" s="138"/>
-      <c r="Z9" s="138"/>
-      <c r="AA9" s="138"/>
+      <c r="R9" s="143"/>
+      <c r="V9" s="140"/>
+      <c r="W9" s="140"/>
+      <c r="X9" s="140"/>
+      <c r="Y9" s="140"/>
+      <c r="Z9" s="140"/>
+      <c r="AA9" s="140"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
@@ -8585,16 +8641,16 @@
       <c r="K10" s="73">
         <v>0</v>
       </c>
-      <c r="L10" s="73">
-        <v>40</v>
+      <c r="L10" s="75">
+        <v>4000</v>
       </c>
       <c r="M10" s="26"/>
-      <c r="V10" s="138"/>
-      <c r="W10" s="138"/>
-      <c r="X10" s="138"/>
-      <c r="Y10" s="138"/>
-      <c r="Z10" s="138"/>
-      <c r="AA10" s="138"/>
+      <c r="V10" s="140"/>
+      <c r="W10" s="140"/>
+      <c r="X10" s="140"/>
+      <c r="Y10" s="140"/>
+      <c r="Z10" s="140"/>
+      <c r="AA10" s="140"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
@@ -8626,15 +8682,15 @@
       <c r="K11" s="73">
         <v>0</v>
       </c>
-      <c r="L11" s="73">
-        <v>40</v>
-      </c>
-      <c r="V11" s="138"/>
-      <c r="W11" s="138"/>
-      <c r="X11" s="138"/>
-      <c r="Y11" s="138"/>
-      <c r="Z11" s="138"/>
-      <c r="AA11" s="138"/>
+      <c r="L11" s="75">
+        <v>4000</v>
+      </c>
+      <c r="V11" s="140"/>
+      <c r="W11" s="140"/>
+      <c r="X11" s="140"/>
+      <c r="Y11" s="140"/>
+      <c r="Z11" s="140"/>
+      <c r="AA11" s="140"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
@@ -8649,51 +8705,51 @@
       <c r="J12" s="49"/>
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
-      <c r="V12" s="138"/>
-      <c r="W12" s="138"/>
-      <c r="X12" s="138"/>
-      <c r="Y12" s="138"/>
-      <c r="Z12" s="138"/>
-      <c r="AA12" s="138"/>
+      <c r="V12" s="140"/>
+      <c r="W12" s="140"/>
+      <c r="X12" s="140"/>
+      <c r="Y12" s="140"/>
+      <c r="Z12" s="140"/>
+      <c r="AA12" s="140"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="Q13" s="49"/>
-      <c r="V13" s="138"/>
-      <c r="W13" s="138"/>
-      <c r="X13" s="138"/>
-      <c r="Y13" s="138"/>
-      <c r="Z13" s="138"/>
-      <c r="AA13" s="138"/>
+      <c r="V13" s="140"/>
+      <c r="W13" s="140"/>
+      <c r="X13" s="140"/>
+      <c r="Y13" s="140"/>
+      <c r="Z13" s="140"/>
+      <c r="AA13" s="140"/>
     </row>
     <row r="14" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="120" t="s">
+      <c r="A14" s="122" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="121"/>
-      <c r="C14" s="121"/>
-      <c r="D14" s="121"/>
-      <c r="E14" s="121"/>
-      <c r="F14" s="121"/>
-      <c r="G14" s="121"/>
-      <c r="H14" s="121"/>
-      <c r="I14" s="121"/>
-      <c r="J14" s="121"/>
-      <c r="K14" s="121"/>
-      <c r="L14" s="121"/>
-      <c r="M14" s="121"/>
-      <c r="N14" s="121"/>
-      <c r="O14" s="121"/>
-      <c r="P14" s="121"/>
+      <c r="B14" s="123"/>
+      <c r="C14" s="123"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="123"/>
+      <c r="I14" s="123"/>
+      <c r="J14" s="123"/>
+      <c r="K14" s="123"/>
+      <c r="L14" s="123"/>
+      <c r="M14" s="123"/>
+      <c r="N14" s="123"/>
+      <c r="O14" s="123"/>
+      <c r="P14" s="123"/>
       <c r="Q14" s="49"/>
       <c r="R14" s="35"/>
       <c r="S14" s="35"/>
       <c r="T14" s="35"/>
-      <c r="V14" s="138"/>
-      <c r="W14" s="138"/>
-      <c r="X14" s="138"/>
-      <c r="Y14" s="138"/>
-      <c r="Z14" s="138"/>
-      <c r="AA14" s="138"/>
+      <c r="V14" s="140"/>
+      <c r="W14" s="140"/>
+      <c r="X14" s="140"/>
+      <c r="Y14" s="140"/>
+      <c r="Z14" s="140"/>
+      <c r="AA14" s="140"/>
     </row>
     <row r="15" spans="1:27" s="35" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
@@ -8711,24 +8767,24 @@
       <c r="E15" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="128" t="s">
+      <c r="F15" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="G15" s="128"/>
-      <c r="H15" s="128"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
       <c r="I15" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="J15" s="135" t="s">
+      <c r="J15" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="136"/>
-      <c r="L15" s="137"/>
-      <c r="M15" s="134" t="s">
+      <c r="K15" s="138"/>
+      <c r="L15" s="139"/>
+      <c r="M15" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="N15" s="134"/>
-      <c r="O15" s="134"/>
+      <c r="N15" s="136"/>
+      <c r="O15" s="136"/>
       <c r="P15" s="36" t="s">
         <v>79</v>
       </c>
@@ -8779,20 +8835,20 @@
       <c r="T17" s="38"/>
     </row>
     <row r="18" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="114" t="s">
+      <c r="A18" s="116" t="s">
         <v>151</v>
       </c>
-      <c r="B18" s="114"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="114"/>
-      <c r="J18" s="114"/>
-      <c r="K18" s="114"/>
-      <c r="L18" s="114"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
+      <c r="G18" s="116"/>
+      <c r="H18" s="116"/>
+      <c r="I18" s="116"/>
+      <c r="J18" s="116"/>
+      <c r="K18" s="116"/>
+      <c r="L18" s="116"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
@@ -8810,16 +8866,16 @@
       <c r="E19" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="79" t="s">
+      <c r="F19" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="85" t="s">
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="J19" s="113"/>
-      <c r="K19" s="86"/>
+      <c r="J19" s="115"/>
+      <c r="K19" s="88"/>
       <c r="L19" s="33" t="s">
         <v>161</v>
       </c>
@@ -8921,7 +8977,7 @@
   <dimension ref="A1:X44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O24:W25"/>
+      <selection activeCell="J25" sqref="F25:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8933,21 +8989,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="116" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="F1" s="80" t="s">
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="F1" s="82" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="82"/>
-      <c r="I1" s="80" t="s">
+      <c r="G1" s="84"/>
+      <c r="I1" s="82" t="s">
         <v>240</v>
       </c>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="82"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="84"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
@@ -8965,12 +9021,12 @@
       <c r="G2" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="138" t="s">
+      <c r="I2" s="140" t="s">
         <v>239</v>
       </c>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="140"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="61"/>
@@ -8982,10 +9038,10 @@
       <c r="G3" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="I3" s="138"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="138"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="140"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="61"/>
@@ -8997,10 +9053,10 @@
       <c r="G4" s="62" t="s">
         <v>167</v>
       </c>
-      <c r="I4" s="138"/>
-      <c r="J4" s="138"/>
-      <c r="K4" s="138"/>
-      <c r="L4" s="138"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="140"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="61"/>
@@ -9012,10 +9068,10 @@
       <c r="G5" s="62" t="s">
         <v>170</v>
       </c>
-      <c r="I5" s="138"/>
-      <c r="J5" s="138"/>
-      <c r="K5" s="138"/>
-      <c r="L5" s="138"/>
+      <c r="I5" s="140"/>
+      <c r="J5" s="140"/>
+      <c r="K5" s="140"/>
+      <c r="L5" s="140"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="61"/>
@@ -9027,10 +9083,10 @@
       <c r="G6" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="I6" s="138"/>
-      <c r="J6" s="138"/>
-      <c r="K6" s="138"/>
-      <c r="L6" s="138"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="140"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="61"/>

</xml_diff>

<commit_message>
commit before integrator change
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/flyball_governor/flyball_governor_gravity_damper.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/flyball_governor/flyball_governor_gravity_damper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\flyball_governor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE0A221-CFFB-4F74-981D-155B7F07840B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B8808A-780A-4D44-85B1-6C4582FBE2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="253">
   <si>
     <t>Mass</t>
   </si>
@@ -1122,7 +1122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1323,24 +1323,102 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1356,79 +1434,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1440,7 +1446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1449,7 +1455,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1461,15 +1473,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1485,15 +1488,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1513,33 +1543,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1975,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B2:Q39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,28 +1998,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="108" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="84"/>
-      <c r="J2" s="80" t="s">
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="110"/>
+      <c r="J2" s="107" t="s">
         <v>157</v>
       </c>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="107"/>
+      <c r="P2" s="107"/>
+      <c r="Q2" s="107"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="77"/>
+      <c r="C3" s="106"/>
       <c r="D3" s="52">
         <v>5</v>
       </c>
@@ -2032,7 +2035,7 @@
         <v>132</v>
       </c>
       <c r="N3" s="79"/>
-      <c r="O3" s="85"/>
+      <c r="O3" s="111"/>
       <c r="P3" s="47" t="s">
         <v>163</v>
       </c>
@@ -2041,10 +2044,10 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="77"/>
+      <c r="C4" s="106"/>
       <c r="D4" s="52">
         <v>2.9999999999999997E-4</v>
       </c>
@@ -2064,7 +2067,7 @@
       <c r="N4" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="O4" s="86"/>
+      <c r="O4" s="112"/>
       <c r="P4" s="47" t="s">
         <v>164</v>
       </c>
@@ -2073,10 +2076,10 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="77"/>
+      <c r="C5" s="106"/>
       <c r="D5" s="52" t="s">
         <v>84</v>
       </c>
@@ -2096,7 +2099,7 @@
       <c r="N5" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="86"/>
+      <c r="O5" s="112"/>
       <c r="P5" s="47" t="s">
         <v>165</v>
       </c>
@@ -2105,10 +2108,10 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="77"/>
+      <c r="C6" s="106"/>
       <c r="D6" s="52" t="s">
         <v>3</v>
       </c>
@@ -2128,7 +2131,7 @@
       <c r="N6" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="O6" s="86"/>
+      <c r="O6" s="112"/>
       <c r="P6" s="47" t="s">
         <v>169</v>
       </c>
@@ -2137,10 +2140,10 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="105" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="77"/>
+      <c r="C7" s="106"/>
       <c r="D7" s="52">
         <v>-9806.65</v>
       </c>
@@ -2160,7 +2163,7 @@
       <c r="N7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="86"/>
+      <c r="O7" s="112"/>
       <c r="P7" s="47" t="s">
         <v>168</v>
       </c>
@@ -2169,10 +2172,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="52" t="s">
         <v>131</v>
       </c>
@@ -2192,7 +2195,7 @@
       <c r="N8" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="86"/>
+      <c r="O8" s="112"/>
       <c r="P8" s="47" t="s">
         <v>172</v>
       </c>
@@ -2201,10 +2204,10 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="105" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="77"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="52"/>
       <c r="E9" s="53" t="s">
         <v>125</v>
@@ -2222,7 +2225,7 @@
       <c r="N9" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="O9" s="86"/>
+      <c r="O9" s="112"/>
       <c r="P9" s="47" t="s">
         <v>173</v>
       </c>
@@ -2244,7 +2247,7 @@
       <c r="N10" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="86"/>
+      <c r="O10" s="112"/>
       <c r="P10" s="51" t="s">
         <v>174</v>
       </c>
@@ -2262,7 +2265,7 @@
       <c r="N11" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="O11" s="86"/>
+      <c r="O11" s="112"/>
       <c r="P11" s="51" t="s">
         <v>175</v>
       </c>
@@ -2271,15 +2274,15 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="107" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
       <c r="J12" s="57"/>
       <c r="K12" s="58"/>
       <c r="L12" s="58"/>
@@ -2289,7 +2292,7 @@
       <c r="N12" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="O12" s="86"/>
+      <c r="O12" s="112"/>
       <c r="P12" s="47" t="s">
         <v>180</v>
       </c>
@@ -2298,19 +2301,19 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="C13" s="81"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="70" t="s">
         <v>241</v>
       </c>
       <c r="E13" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
       <c r="J13" s="57"/>
       <c r="K13" s="58"/>
       <c r="L13" s="58"/>
@@ -2320,7 +2323,7 @@
       <c r="N13" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="86"/>
+      <c r="O13" s="112"/>
       <c r="P13" s="51" t="s">
         <v>181</v>
       </c>
@@ -2329,19 +2332,19 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="81"/>
+      <c r="C14" s="77"/>
       <c r="D14" s="70" t="s">
         <v>241</v>
       </c>
       <c r="E14" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="F14" s="111"/>
-      <c r="G14" s="111"/>
-      <c r="H14" s="111"/>
+      <c r="F14" s="104"/>
+      <c r="G14" s="104"/>
+      <c r="H14" s="104"/>
       <c r="J14" s="59"/>
       <c r="K14" s="60"/>
       <c r="L14" s="58"/>
@@ -2351,7 +2354,7 @@
       <c r="N14" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="O14" s="86"/>
+      <c r="O14" s="112"/>
       <c r="P14" s="51" t="s">
         <v>182</v>
       </c>
@@ -2360,17 +2363,17 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="81"/>
+      <c r="C15" s="77"/>
       <c r="D15" s="70"/>
       <c r="E15" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="F15" s="111"/>
-      <c r="G15" s="111"/>
-      <c r="H15" s="111"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="104"/>
+      <c r="H15" s="104"/>
       <c r="J15" s="78" t="s">
         <v>95</v>
       </c>
@@ -2382,7 +2385,7 @@
       <c r="N15" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="86"/>
+      <c r="O15" s="112"/>
       <c r="P15" s="51" t="s">
         <v>183</v>
       </c>
@@ -2391,19 +2394,19 @@
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="77" t="s">
         <v>148</v>
       </c>
-      <c r="C16" s="81"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="70" t="s">
         <v>241</v>
       </c>
       <c r="E16" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="F16" s="111"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="111"/>
+      <c r="F16" s="104"/>
+      <c r="G16" s="104"/>
+      <c r="H16" s="104"/>
       <c r="J16" s="47" t="s">
         <v>96</v>
       </c>
@@ -2417,7 +2420,7 @@
       <c r="N16" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="O16" s="86"/>
+      <c r="O16" s="112"/>
       <c r="P16" s="47" t="s">
         <v>188</v>
       </c>
@@ -2426,17 +2429,17 @@
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="81"/>
+      <c r="C17" s="77"/>
       <c r="D17" s="70"/>
       <c r="E17" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="F17" s="111"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="111"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="104"/>
       <c r="J17" s="47" t="s">
         <v>0</v>
       </c>
@@ -2448,7 +2451,7 @@
         <v>152</v>
       </c>
       <c r="N17" s="79"/>
-      <c r="O17" s="86"/>
+      <c r="O17" s="112"/>
       <c r="P17" s="51" t="s">
         <v>189</v>
       </c>
@@ -2457,19 +2460,19 @@
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="98" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="88"/>
+      <c r="C18" s="99"/>
       <c r="D18" s="46" t="s">
         <v>241</v>
       </c>
       <c r="E18" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="104"/>
       <c r="J18" s="47" t="s">
         <v>97</v>
       </c>
@@ -2483,7 +2486,7 @@
       <c r="N18" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="O18" s="86"/>
+      <c r="O18" s="112"/>
       <c r="P18" s="51" t="s">
         <v>190</v>
       </c>
@@ -2492,17 +2495,17 @@
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="88"/>
+      <c r="C19" s="99"/>
       <c r="D19" s="46"/>
       <c r="E19" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="111"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
       <c r="J19" s="47" t="s">
         <v>98</v>
       </c>
@@ -2516,7 +2519,7 @@
       <c r="N19" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="O19" s="86"/>
+      <c r="O19" s="112"/>
       <c r="P19" s="51" t="s">
         <v>191</v>
       </c>
@@ -2525,19 +2528,19 @@
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="109" t="s">
+      <c r="B20" s="102" t="s">
         <v>251</v>
       </c>
-      <c r="C20" s="110"/>
+      <c r="C20" s="103"/>
       <c r="D20" s="50" t="s">
         <v>241</v>
       </c>
       <c r="E20" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="111"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="104"/>
       <c r="J20" s="47" t="s">
         <v>104</v>
       </c>
@@ -2551,7 +2554,7 @@
       <c r="N20" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="O20" s="86"/>
+      <c r="O20" s="112"/>
       <c r="P20" s="47" t="s">
         <v>196</v>
       </c>
@@ -2560,17 +2563,17 @@
       </c>
     </row>
     <row r="21" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="77" t="s">
         <v>252</v>
       </c>
-      <c r="C21" s="81"/>
+      <c r="C21" s="77"/>
       <c r="D21" s="71"/>
       <c r="E21" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="F21" s="111"/>
-      <c r="G21" s="111"/>
-      <c r="H21" s="111"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="104"/>
       <c r="J21" s="47" t="s">
         <v>99</v>
       </c>
@@ -2584,7 +2587,7 @@
       <c r="N21" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="O21" s="86"/>
+      <c r="O21" s="112"/>
       <c r="P21" s="51" t="s">
         <v>197</v>
       </c>
@@ -2593,21 +2596,21 @@
       </c>
     </row>
     <row r="22" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="92" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="102"/>
+      <c r="C22" s="93"/>
       <c r="D22" s="44">
         <v>2</v>
       </c>
-      <c r="E22" s="98" t="s">
+      <c r="E22" s="89" t="s">
         <v>149</v>
       </c>
-      <c r="F22" s="89" t="s">
+      <c r="F22" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="G22" s="90"/>
-      <c r="H22" s="91"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="82"/>
       <c r="J22" s="32" t="s">
         <v>110</v>
       </c>
@@ -2621,7 +2624,7 @@
       <c r="N22" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="O22" s="86"/>
+      <c r="O22" s="112"/>
       <c r="P22" s="51" t="s">
         <v>198</v>
       </c>
@@ -2630,19 +2633,19 @@
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="103"/>
-      <c r="C23" s="104"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="95"/>
       <c r="D23" s="44"/>
-      <c r="E23" s="99"/>
-      <c r="F23" s="92"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="94"/>
-      <c r="J23" s="107"/>
-      <c r="K23" s="107"/>
-      <c r="L23" s="107"/>
-      <c r="M23" s="107"/>
-      <c r="N23" s="108"/>
-      <c r="O23" s="86"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="85"/>
+      <c r="J23" s="100"/>
+      <c r="K23" s="100"/>
+      <c r="L23" s="100"/>
+      <c r="M23" s="100"/>
+      <c r="N23" s="101"/>
+      <c r="O23" s="112"/>
       <c r="P23" s="51" t="s">
         <v>199</v>
       </c>
@@ -2651,19 +2654,19 @@
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="103"/>
-      <c r="C24" s="104"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="95"/>
       <c r="D24" s="44"/>
-      <c r="E24" s="99"/>
-      <c r="F24" s="92"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="94"/>
-      <c r="J24" s="107"/>
-      <c r="K24" s="107"/>
-      <c r="L24" s="107"/>
-      <c r="M24" s="107"/>
-      <c r="N24" s="108"/>
-      <c r="O24" s="86"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="84"/>
+      <c r="H24" s="85"/>
+      <c r="J24" s="100"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="100"/>
+      <c r="M24" s="100"/>
+      <c r="N24" s="101"/>
+      <c r="O24" s="112"/>
       <c r="P24" s="32" t="s">
         <v>205</v>
       </c>
@@ -2672,19 +2675,19 @@
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="103"/>
-      <c r="C25" s="104"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="95"/>
       <c r="D25" s="44"/>
-      <c r="E25" s="99"/>
-      <c r="F25" s="92"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="94"/>
-      <c r="J25" s="107"/>
-      <c r="K25" s="107"/>
-      <c r="L25" s="107"/>
-      <c r="M25" s="107"/>
-      <c r="N25" s="108"/>
-      <c r="O25" s="86"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="85"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="101"/>
+      <c r="O25" s="112"/>
       <c r="P25" s="32" t="s">
         <v>209</v>
       </c>
@@ -2693,19 +2696,19 @@
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="103"/>
-      <c r="C26" s="104"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="95"/>
       <c r="D26" s="44"/>
-      <c r="E26" s="99"/>
-      <c r="F26" s="92"/>
-      <c r="G26" s="93"/>
-      <c r="H26" s="94"/>
-      <c r="J26" s="107"/>
-      <c r="K26" s="107"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="107"/>
-      <c r="N26" s="108"/>
-      <c r="O26" s="86"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="84"/>
+      <c r="H26" s="85"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="100"/>
+      <c r="M26" s="100"/>
+      <c r="N26" s="101"/>
+      <c r="O26" s="112"/>
       <c r="P26" s="32" t="s">
         <v>210</v>
       </c>
@@ -2714,19 +2717,19 @@
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="103"/>
-      <c r="C27" s="104"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="95"/>
       <c r="D27" s="44"/>
-      <c r="E27" s="99"/>
-      <c r="F27" s="92"/>
-      <c r="G27" s="93"/>
-      <c r="H27" s="94"/>
-      <c r="J27" s="107"/>
-      <c r="K27" s="107"/>
-      <c r="L27" s="107"/>
-      <c r="M27" s="107"/>
-      <c r="N27" s="108"/>
-      <c r="O27" s="86"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="84"/>
+      <c r="H27" s="85"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="100"/>
+      <c r="N27" s="101"/>
+      <c r="O27" s="112"/>
       <c r="P27" s="32" t="s">
         <v>211</v>
       </c>
@@ -2735,19 +2738,19 @@
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="103"/>
-      <c r="C28" s="104"/>
+      <c r="B28" s="94"/>
+      <c r="C28" s="95"/>
       <c r="D28" s="44"/>
-      <c r="E28" s="99"/>
-      <c r="F28" s="92"/>
-      <c r="G28" s="93"/>
-      <c r="H28" s="94"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="107"/>
-      <c r="L28" s="107"/>
-      <c r="M28" s="107"/>
-      <c r="N28" s="108"/>
-      <c r="O28" s="86"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="85"/>
+      <c r="J28" s="100"/>
+      <c r="K28" s="100"/>
+      <c r="L28" s="100"/>
+      <c r="M28" s="100"/>
+      <c r="N28" s="101"/>
+      <c r="O28" s="112"/>
       <c r="P28" s="32" t="s">
         <v>213</v>
       </c>
@@ -2756,19 +2759,19 @@
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="105"/>
-      <c r="C29" s="106"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="97"/>
       <c r="D29" s="44"/>
-      <c r="E29" s="100"/>
-      <c r="F29" s="95"/>
-      <c r="G29" s="96"/>
-      <c r="H29" s="97"/>
-      <c r="J29" s="107"/>
-      <c r="K29" s="107"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="107"/>
-      <c r="N29" s="108"/>
-      <c r="O29" s="86"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="88"/>
+      <c r="J29" s="100"/>
+      <c r="K29" s="100"/>
+      <c r="L29" s="100"/>
+      <c r="M29" s="100"/>
+      <c r="N29" s="101"/>
+      <c r="O29" s="112"/>
       <c r="P29" s="32" t="s">
         <v>212</v>
       </c>
@@ -2777,12 +2780,12 @@
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J30" s="107"/>
-      <c r="K30" s="107"/>
-      <c r="L30" s="107"/>
-      <c r="M30" s="107"/>
-      <c r="N30" s="108"/>
-      <c r="O30" s="86"/>
+      <c r="J30" s="100"/>
+      <c r="K30" s="100"/>
+      <c r="L30" s="100"/>
+      <c r="M30" s="100"/>
+      <c r="N30" s="101"/>
+      <c r="O30" s="112"/>
       <c r="P30" s="32" t="s">
         <v>214</v>
       </c>
@@ -2791,12 +2794,12 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J31" s="107"/>
-      <c r="K31" s="107"/>
-      <c r="L31" s="107"/>
-      <c r="M31" s="107"/>
-      <c r="N31" s="108"/>
-      <c r="O31" s="86"/>
+      <c r="J31" s="100"/>
+      <c r="K31" s="100"/>
+      <c r="L31" s="100"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="101"/>
+      <c r="O31" s="112"/>
       <c r="P31" s="32" t="s">
         <v>215</v>
       </c>
@@ -2805,12 +2808,12 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J32" s="107"/>
-      <c r="K32" s="107"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="107"/>
-      <c r="N32" s="108"/>
-      <c r="O32" s="86"/>
+      <c r="J32" s="100"/>
+      <c r="K32" s="100"/>
+      <c r="L32" s="100"/>
+      <c r="M32" s="100"/>
+      <c r="N32" s="101"/>
+      <c r="O32" s="112"/>
       <c r="P32" s="32" t="s">
         <v>216</v>
       </c>
@@ -2819,12 +2822,12 @@
       </c>
     </row>
     <row r="33" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J33" s="107"/>
-      <c r="K33" s="107"/>
-      <c r="L33" s="107"/>
-      <c r="M33" s="107"/>
-      <c r="N33" s="108"/>
-      <c r="O33" s="86"/>
+      <c r="J33" s="100"/>
+      <c r="K33" s="100"/>
+      <c r="L33" s="100"/>
+      <c r="M33" s="100"/>
+      <c r="N33" s="101"/>
+      <c r="O33" s="112"/>
       <c r="P33" s="32" t="s">
         <v>217</v>
       </c>
@@ -2833,12 +2836,12 @@
       </c>
     </row>
     <row r="34" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J34" s="107"/>
-      <c r="K34" s="107"/>
-      <c r="L34" s="107"/>
-      <c r="M34" s="107"/>
-      <c r="N34" s="108"/>
-      <c r="O34" s="86"/>
+      <c r="J34" s="100"/>
+      <c r="K34" s="100"/>
+      <c r="L34" s="100"/>
+      <c r="M34" s="100"/>
+      <c r="N34" s="101"/>
+      <c r="O34" s="112"/>
       <c r="P34" s="32" t="s">
         <v>218</v>
       </c>
@@ -2847,12 +2850,12 @@
       </c>
     </row>
     <row r="35" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J35" s="107"/>
-      <c r="K35" s="107"/>
-      <c r="L35" s="107"/>
-      <c r="M35" s="107"/>
-      <c r="N35" s="108"/>
-      <c r="O35" s="86"/>
+      <c r="J35" s="100"/>
+      <c r="K35" s="100"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="100"/>
+      <c r="N35" s="101"/>
+      <c r="O35" s="112"/>
       <c r="P35" s="32" t="s">
         <v>219</v>
       </c>
@@ -2861,12 +2864,12 @@
       </c>
     </row>
     <row r="36" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J36" s="107"/>
-      <c r="K36" s="107"/>
-      <c r="L36" s="107"/>
-      <c r="M36" s="107"/>
-      <c r="N36" s="108"/>
-      <c r="O36" s="86"/>
+      <c r="J36" s="100"/>
+      <c r="K36" s="100"/>
+      <c r="L36" s="100"/>
+      <c r="M36" s="100"/>
+      <c r="N36" s="101"/>
+      <c r="O36" s="112"/>
       <c r="P36" s="32" t="s">
         <v>228</v>
       </c>
@@ -2875,12 +2878,12 @@
       </c>
     </row>
     <row r="37" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J37" s="107"/>
-      <c r="K37" s="107"/>
-      <c r="L37" s="107"/>
-      <c r="M37" s="107"/>
-      <c r="N37" s="108"/>
-      <c r="O37" s="86"/>
+      <c r="J37" s="100"/>
+      <c r="K37" s="100"/>
+      <c r="L37" s="100"/>
+      <c r="M37" s="100"/>
+      <c r="N37" s="101"/>
+      <c r="O37" s="112"/>
       <c r="P37" s="32" t="s">
         <v>229</v>
       </c>
@@ -2889,12 +2892,12 @@
       </c>
     </row>
     <row r="38" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J38" s="107"/>
-      <c r="K38" s="107"/>
-      <c r="L38" s="107"/>
-      <c r="M38" s="107"/>
-      <c r="N38" s="108"/>
-      <c r="O38" s="86"/>
+      <c r="J38" s="100"/>
+      <c r="K38" s="100"/>
+      <c r="L38" s="100"/>
+      <c r="M38" s="100"/>
+      <c r="N38" s="101"/>
+      <c r="O38" s="112"/>
       <c r="P38" s="32" t="s">
         <v>230</v>
       </c>
@@ -2903,12 +2906,12 @@
       </c>
     </row>
     <row r="39" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J39" s="107"/>
-      <c r="K39" s="107"/>
-      <c r="L39" s="107"/>
-      <c r="M39" s="107"/>
-      <c r="N39" s="108"/>
-      <c r="O39" s="86"/>
+      <c r="J39" s="100"/>
+      <c r="K39" s="100"/>
+      <c r="L39" s="100"/>
+      <c r="M39" s="100"/>
+      <c r="N39" s="101"/>
+      <c r="O39" s="112"/>
       <c r="P39" s="32" t="s">
         <v>231</v>
       </c>
@@ -2918,19 +2921,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="F22:H29"/>
-    <mergeCell ref="E22:E29"/>
-    <mergeCell ref="B22:C29"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="J23:N39"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F13:H21"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="M3:N3"/>
@@ -2947,6 +2937,19 @@
     <mergeCell ref="O3:O39"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="F22:H29"/>
+    <mergeCell ref="E22:E29"/>
+    <mergeCell ref="B22:C29"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="J23:N39"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F13:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2978,118 +2981,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="111"/>
-      <c r="B1" s="111"/>
-      <c r="C1" s="81" t="s">
+      <c r="A1" s="104"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81" t="s">
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81" t="s">
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81" t="s">
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
-      <c r="S1" s="81" t="s">
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="81"/>
-      <c r="U1" s="81"/>
-      <c r="V1" s="81"/>
-      <c r="W1" s="81"/>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="81"/>
-      <c r="Z1" s="81"/>
-      <c r="AA1" s="81"/>
-      <c r="AB1" s="81"/>
-      <c r="AC1" s="81"/>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="81"/>
-      <c r="AF1" s="81"/>
-      <c r="AG1" s="81"/>
-      <c r="AH1" s="81"/>
-      <c r="AI1" s="81"/>
-      <c r="AJ1" s="81"/>
-      <c r="AK1" s="81"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="111"/>
-      <c r="B2" s="111"/>
-      <c r="C2" s="113" t="s">
+      <c r="A2" s="104"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113" t="s">
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113" t="s">
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="81" t="s">
+      <c r="J2" s="115"/>
+      <c r="K2" s="115"/>
+      <c r="L2" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81" t="s">
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="114" t="s">
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="S2" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="113" t="s">
+      <c r="S2" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="81" t="s">
+      <c r="U2" s="115"/>
+      <c r="V2" s="115"/>
+      <c r="W2" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="X2" s="81"/>
-      <c r="Y2" s="81"/>
-      <c r="Z2" s="87" t="s">
+      <c r="X2" s="77"/>
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="98" t="s">
         <v>93</v>
       </c>
-      <c r="AA2" s="115"/>
-      <c r="AB2" s="88"/>
-      <c r="AC2" s="81" t="s">
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="99"/>
+      <c r="AC2" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="AD2" s="81"/>
-      <c r="AE2" s="81"/>
-      <c r="AF2" s="81" t="s">
+      <c r="AD2" s="77"/>
+      <c r="AE2" s="77"/>
+      <c r="AF2" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="AG2" s="81"/>
-      <c r="AH2" s="81"/>
-      <c r="AI2" s="81" t="s">
+      <c r="AG2" s="77"/>
+      <c r="AH2" s="77"/>
+      <c r="AI2" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="AJ2" s="81"/>
-      <c r="AK2" s="81"/>
+      <c r="AJ2" s="77"/>
+      <c r="AK2" s="77"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -3143,8 +3146,8 @@
       <c r="Q3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="114"/>
-      <c r="S3" s="112"/>
+      <c r="R3" s="116"/>
+      <c r="S3" s="114"/>
       <c r="T3" s="16" t="s">
         <v>62</v>
       </c>
@@ -6829,12 +6832,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -6848,6 +6845,12 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6879,16 +6882,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -6919,11 +6922,11 @@
       <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="117" t="s">
+      <c r="F2" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -6979,19 +6982,19 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="116"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="116"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="118"/>
+      <c r="K5" s="118"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -7016,16 +7019,16 @@
       <c r="E6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="119" t="s">
+      <c r="F6" s="123" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="120"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="119" t="s">
+      <c r="G6" s="124"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="120"/>
-      <c r="K6" s="121"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="125"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="20"/>
@@ -7061,22 +7064,22 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="116"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="116"/>
-      <c r="M8" s="116"/>
-      <c r="N8" s="116"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="118"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -7101,21 +7104,21 @@
       <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="117" t="s">
+      <c r="F9" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="117"/>
-      <c r="H9" s="117"/>
-      <c r="I9" s="118" t="s">
+      <c r="G9" s="119"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="118"/>
-      <c r="K9" s="118"/>
-      <c r="L9" s="118" t="s">
+      <c r="J9" s="117"/>
+      <c r="K9" s="117"/>
+      <c r="L9" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="M9" s="118"/>
-      <c r="N9" s="118"/>
+      <c r="M9" s="117"/>
+      <c r="N9" s="117"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -7169,19 +7172,19 @@
       <c r="X11" s="10"/>
     </row>
     <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="116"/>
-      <c r="K12" s="116"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="118"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
@@ -7206,16 +7209,16 @@
       <c r="E13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="117" t="s">
+      <c r="F13" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="117"/>
-      <c r="H13" s="117"/>
-      <c r="I13" s="118" t="s">
+      <c r="G13" s="119"/>
+      <c r="H13" s="119"/>
+      <c r="I13" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="118"/>
-      <c r="K13" s="118"/>
+      <c r="J13" s="117"/>
+      <c r="K13" s="117"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -7357,19 +7360,19 @@
       <c r="X17" s="10"/>
     </row>
     <row r="18" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="116" t="s">
+      <c r="A18" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="116"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="116"/>
-      <c r="F18" s="116"/>
-      <c r="G18" s="116"/>
-      <c r="H18" s="116"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="116"/>
-      <c r="K18" s="116"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="118"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
@@ -7394,16 +7397,16 @@
       <c r="E19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="117" t="s">
+      <c r="F19" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="117"/>
-      <c r="H19" s="117"/>
-      <c r="I19" s="118" t="s">
+      <c r="G19" s="119"/>
+      <c r="H19" s="119"/>
+      <c r="I19" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="118"/>
-      <c r="K19" s="118"/>
+      <c r="J19" s="117"/>
+      <c r="K19" s="117"/>
     </row>
     <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -7440,19 +7443,19 @@
       <c r="X21" s="10"/>
     </row>
     <row r="22" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="116"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116"/>
-      <c r="I22" s="116"/>
-      <c r="J22" s="116"/>
-      <c r="K22" s="116"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="118"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
@@ -7477,16 +7480,16 @@
       <c r="E23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="117" t="s">
+      <c r="F23" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="117"/>
-      <c r="H23" s="117"/>
-      <c r="I23" s="118" t="s">
+      <c r="G23" s="119"/>
+      <c r="H23" s="119"/>
+      <c r="I23" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="118"/>
-      <c r="K23" s="118"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="117"/>
     </row>
     <row r="24" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
@@ -7523,22 +7526,22 @@
     </row>
     <row r="25" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="118" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="116"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="116"/>
-      <c r="J26" s="116"/>
-      <c r="K26" s="116"/>
-      <c r="L26" s="116"/>
-      <c r="M26" s="116"/>
-      <c r="N26" s="116"/>
+      <c r="B26" s="118"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="118"/>
+      <c r="H26" s="118"/>
+      <c r="I26" s="118"/>
+      <c r="J26" s="118"/>
+      <c r="K26" s="118"/>
+      <c r="L26" s="118"/>
+      <c r="M26" s="118"/>
+      <c r="N26" s="118"/>
     </row>
     <row r="27" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
@@ -7556,44 +7559,44 @@
       <c r="E27" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="117" t="s">
+      <c r="F27" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="G27" s="117"/>
-      <c r="H27" s="117"/>
-      <c r="I27" s="118" t="s">
+      <c r="G27" s="119"/>
+      <c r="H27" s="119"/>
+      <c r="I27" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="118"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="118" t="s">
+      <c r="J27" s="117"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="117" t="s">
         <v>127</v>
       </c>
-      <c r="M27" s="118"/>
-      <c r="N27" s="118"/>
+      <c r="M27" s="117"/>
+      <c r="N27" s="117"/>
     </row>
     <row r="28" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="116" t="s">
+      <c r="A30" s="118" t="s">
         <v>128</v>
       </c>
-      <c r="B30" s="116"/>
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
-      <c r="E30" s="116"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
-      <c r="H30" s="116"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="116"/>
-      <c r="K30" s="116"/>
-      <c r="L30" s="116"/>
-      <c r="M30" s="116"/>
-      <c r="N30" s="116"/>
-      <c r="O30" s="116"/>
-      <c r="P30" s="116"/>
-      <c r="Q30" s="116"/>
+      <c r="B30" s="118"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="118"/>
+      <c r="F30" s="118"/>
+      <c r="G30" s="118"/>
+      <c r="H30" s="118"/>
+      <c r="I30" s="118"/>
+      <c r="J30" s="118"/>
+      <c r="K30" s="118"/>
+      <c r="L30" s="118"/>
+      <c r="M30" s="118"/>
+      <c r="N30" s="118"/>
+      <c r="O30" s="118"/>
+      <c r="P30" s="118"/>
+      <c r="Q30" s="118"/>
     </row>
     <row r="31" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
@@ -7611,26 +7614,26 @@
       <c r="E31" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="119" t="s">
+      <c r="F31" s="123" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="120"/>
-      <c r="H31" s="121"/>
-      <c r="I31" s="119" t="s">
+      <c r="G31" s="124"/>
+      <c r="H31" s="125"/>
+      <c r="I31" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="120"/>
-      <c r="K31" s="121"/>
-      <c r="L31" s="118" t="s">
+      <c r="J31" s="124"/>
+      <c r="K31" s="125"/>
+      <c r="L31" s="117" t="s">
         <v>129</v>
       </c>
-      <c r="M31" s="118"/>
-      <c r="N31" s="118"/>
-      <c r="O31" s="118" t="s">
+      <c r="M31" s="117"/>
+      <c r="N31" s="117"/>
+      <c r="O31" s="117" t="s">
         <v>130</v>
       </c>
-      <c r="P31" s="118"/>
-      <c r="Q31" s="118"/>
+      <c r="P31" s="117"/>
+      <c r="Q31" s="117"/>
     </row>
     <row r="32" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
@@ -7653,14 +7656,14 @@
     </row>
     <row r="33" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="116" t="s">
+      <c r="A34" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="116"/>
-      <c r="C34" s="116"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="116"/>
-      <c r="F34" s="116"/>
+      <c r="B34" s="118"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="118"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
@@ -7738,12 +7741,12 @@
       <c r="X37" s="10"/>
     </row>
     <row r="38" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="116" t="s">
+      <c r="A38" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="116"/>
-      <c r="C38" s="116"/>
-      <c r="D38" s="116"/>
+      <c r="B38" s="118"/>
+      <c r="C38" s="118"/>
+      <c r="D38" s="118"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -7836,15 +7839,15 @@
       <c r="Q41" s="10"/>
     </row>
     <row r="42" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="122" t="s">
+      <c r="A42" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="123"/>
-      <c r="C42" s="123"/>
-      <c r="D42" s="123"/>
-      <c r="E42" s="123"/>
-      <c r="F42" s="123"/>
-      <c r="G42" s="124"/>
+      <c r="B42" s="121"/>
+      <c r="C42" s="121"/>
+      <c r="D42" s="121"/>
+      <c r="E42" s="121"/>
+      <c r="F42" s="121"/>
+      <c r="G42" s="122"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -7868,11 +7871,11 @@
       <c r="D43" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="118" t="s">
+      <c r="E43" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="F43" s="118"/>
-      <c r="G43" s="118"/>
+      <c r="F43" s="117"/>
+      <c r="G43" s="117"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -8139,6 +8142,21 @@
     <row r="65" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
     <mergeCell ref="E43:G43"/>
     <mergeCell ref="A22:K22"/>
     <mergeCell ref="F23:H23"/>
@@ -8155,21 +8173,6 @@
     <mergeCell ref="I31:K31"/>
     <mergeCell ref="L31:N31"/>
     <mergeCell ref="O31:Q31"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A8:N8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -8205,18 +8208,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="129"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -8234,11 +8237,11 @@
       <c r="E2" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="125" t="s">
+      <c r="F2" s="126" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="126"/>
-      <c r="H2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="128"/>
       <c r="I2" s="25" t="s">
         <v>49</v>
       </c>
@@ -8267,8 +8270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F55610B-D925-4735-AE3D-EBBD0AD81ACC}">
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8291,58 +8294,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="140" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="132"/>
-      <c r="R1" s="132"/>
-      <c r="S1" s="132"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
+      <c r="O1" s="141"/>
+      <c r="P1" s="141"/>
+      <c r="Q1" s="141"/>
+      <c r="R1" s="141"/>
+      <c r="S1" s="141"/>
     </row>
     <row r="2" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="116"/>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="133" t="s">
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="O2" s="134"/>
-      <c r="P2" s="134"/>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="134"/>
-      <c r="S2" s="135"/>
-      <c r="V2" s="140" t="s">
+      <c r="O2" s="144"/>
+      <c r="P2" s="144"/>
+      <c r="Q2" s="144"/>
+      <c r="R2" s="144"/>
+      <c r="S2" s="145"/>
+      <c r="V2" s="131" t="s">
         <v>123</v>
       </c>
-      <c r="W2" s="140"/>
-      <c r="X2" s="140"/>
-      <c r="Y2" s="140"/>
-      <c r="Z2" s="140"/>
-      <c r="AA2" s="140"/>
+      <c r="W2" s="131"/>
+      <c r="X2" s="131"/>
+      <c r="Y2" s="131"/>
+      <c r="Z2" s="131"/>
+      <c r="AA2" s="131"/>
     </row>
     <row r="3" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
@@ -8360,16 +8363,16 @@
       <c r="E3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="141" t="s">
+      <c r="F3" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="142"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="145" t="s">
+      <c r="G3" s="133"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="146"/>
-      <c r="K3" s="147"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="138"/>
       <c r="L3" s="66" t="s">
         <v>249</v>
       </c>
@@ -8388,176 +8391,132 @@
       <c r="Q3" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="R3" s="144" t="s">
+      <c r="R3" s="135" t="s">
         <v>122</v>
       </c>
-      <c r="S3" s="144"/>
-      <c r="V3" s="140"/>
-      <c r="W3" s="140"/>
-      <c r="X3" s="140"/>
-      <c r="Y3" s="140"/>
-      <c r="Z3" s="140"/>
-      <c r="AA3" s="140"/>
+      <c r="S3" s="135"/>
+      <c r="V3" s="131"/>
+      <c r="W3" s="131"/>
+      <c r="X3" s="131"/>
+      <c r="Y3" s="131"/>
+      <c r="Z3" s="131"/>
+      <c r="AA3" s="131"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="74" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74">
-        <v>2</v>
-      </c>
-      <c r="E4" s="74">
-        <v>4</v>
-      </c>
-      <c r="F4" s="74">
-        <v>-50</v>
-      </c>
-      <c r="G4" s="74">
-        <v>500</v>
-      </c>
-      <c r="H4" s="74">
-        <v>0</v>
-      </c>
-      <c r="I4" s="74">
-        <v>-460</v>
-      </c>
-      <c r="J4" s="74">
-        <v>750</v>
-      </c>
-      <c r="K4" s="74">
-        <v>0</v>
-      </c>
-      <c r="L4" s="74">
-        <v>500</v>
-      </c>
-      <c r="M4" s="18">
-        <v>800</v>
-      </c>
+      <c r="B4" s="74"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
       <c r="N4" s="41"/>
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
-      <c r="V4" s="140"/>
-      <c r="W4" s="140"/>
-      <c r="X4" s="140"/>
-      <c r="Y4" s="140"/>
-      <c r="Z4" s="140"/>
-      <c r="AA4" s="140"/>
+      <c r="V4" s="131"/>
+      <c r="W4" s="131"/>
+      <c r="X4" s="131"/>
+      <c r="Y4" s="131"/>
+      <c r="Z4" s="131"/>
+      <c r="AA4" s="131"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="74"/>
-      <c r="B5" s="74" t="s">
-        <v>72</v>
-      </c>
+      <c r="B5" s="74"/>
       <c r="C5" s="74"/>
-      <c r="D5" s="74">
-        <v>2</v>
-      </c>
-      <c r="E5" s="74">
-        <v>5</v>
-      </c>
-      <c r="F5" s="74">
-        <v>50</v>
-      </c>
-      <c r="G5" s="74">
-        <v>500</v>
-      </c>
-      <c r="H5" s="74">
-        <v>0</v>
-      </c>
-      <c r="I5" s="74">
-        <v>460</v>
-      </c>
-      <c r="J5" s="74">
-        <v>750</v>
-      </c>
-      <c r="K5" s="74">
-        <v>0</v>
-      </c>
-      <c r="L5" s="74">
-        <v>500</v>
-      </c>
-      <c r="M5" s="18">
-        <v>800</v>
-      </c>
-      <c r="N5" s="49"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
       <c r="O5" s="49"/>
       <c r="P5" s="49"/>
       <c r="Q5" s="49"/>
       <c r="R5" s="49"/>
       <c r="S5" s="49"/>
-      <c r="V5" s="140"/>
-      <c r="W5" s="140"/>
-      <c r="X5" s="140"/>
-      <c r="Y5" s="140"/>
-      <c r="Z5" s="140"/>
-      <c r="AA5" s="140"/>
+      <c r="V5" s="131"/>
+      <c r="W5" s="131"/>
+      <c r="X5" s="131"/>
+      <c r="Y5" s="131"/>
+      <c r="Z5" s="131"/>
+      <c r="AA5" s="131"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V6" s="140"/>
-      <c r="W6" s="140"/>
-      <c r="X6" s="140"/>
-      <c r="Y6" s="140"/>
-      <c r="Z6" s="140"/>
-      <c r="AA6" s="140"/>
+      <c r="V6" s="131"/>
+      <c r="W6" s="131"/>
+      <c r="X6" s="131"/>
+      <c r="Y6" s="131"/>
+      <c r="Z6" s="131"/>
+      <c r="AA6" s="131"/>
     </row>
     <row r="7" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="131" t="s">
+      <c r="A7" s="140" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="132"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="132"/>
-      <c r="J7" s="132"/>
-      <c r="K7" s="132"/>
-      <c r="L7" s="132"/>
-      <c r="M7" s="132"/>
-      <c r="N7" s="132"/>
-      <c r="O7" s="132"/>
-      <c r="P7" s="132"/>
-      <c r="Q7" s="132"/>
-      <c r="R7" s="132"/>
-      <c r="V7" s="140"/>
-      <c r="W7" s="140"/>
-      <c r="X7" s="140"/>
-      <c r="Y7" s="140"/>
-      <c r="Z7" s="140"/>
-      <c r="AA7" s="140"/>
+      <c r="B7" s="141"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="141"/>
+      <c r="E7" s="141"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="141"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="141"/>
+      <c r="N7" s="141"/>
+      <c r="O7" s="141"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="141"/>
+      <c r="R7" s="141"/>
+      <c r="V7" s="131"/>
+      <c r="W7" s="131"/>
+      <c r="X7" s="131"/>
+      <c r="Y7" s="131"/>
+      <c r="Z7" s="131"/>
+      <c r="AA7" s="131"/>
     </row>
     <row r="8" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="116"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="116"/>
-      <c r="M8" s="116"/>
-      <c r="N8" s="148" t="s">
+      <c r="A8" s="118"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="139" t="s">
         <v>119</v>
       </c>
-      <c r="O8" s="148"/>
-      <c r="P8" s="148"/>
-      <c r="Q8" s="148"/>
-      <c r="R8" s="148"/>
-      <c r="V8" s="140"/>
-      <c r="W8" s="140"/>
-      <c r="X8" s="140"/>
-      <c r="Y8" s="140"/>
-      <c r="Z8" s="140"/>
-      <c r="AA8" s="140"/>
+      <c r="O8" s="139"/>
+      <c r="P8" s="139"/>
+      <c r="Q8" s="139"/>
+      <c r="R8" s="139"/>
+      <c r="V8" s="131"/>
+      <c r="W8" s="131"/>
+      <c r="X8" s="131"/>
+      <c r="Y8" s="131"/>
+      <c r="Z8" s="131"/>
+      <c r="AA8" s="131"/>
     </row>
     <row r="9" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
@@ -8575,16 +8534,16 @@
       <c r="E9" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="141" t="s">
+      <c r="F9" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="142"/>
-      <c r="H9" s="143"/>
-      <c r="I9" s="145" t="s">
+      <c r="G9" s="133"/>
+      <c r="H9" s="134"/>
+      <c r="I9" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="146"/>
-      <c r="K9" s="147"/>
+      <c r="J9" s="137"/>
+      <c r="K9" s="138"/>
       <c r="L9" s="40" t="s">
         <v>114</v>
       </c>
@@ -8600,16 +8559,16 @@
       <c r="P9" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="Q9" s="141" t="s">
+      <c r="Q9" s="132" t="s">
         <v>121</v>
       </c>
-      <c r="R9" s="143"/>
-      <c r="V9" s="140"/>
-      <c r="W9" s="140"/>
-      <c r="X9" s="140"/>
-      <c r="Y9" s="140"/>
-      <c r="Z9" s="140"/>
-      <c r="AA9" s="140"/>
+      <c r="R9" s="134"/>
+      <c r="V9" s="131"/>
+      <c r="W9" s="131"/>
+      <c r="X9" s="131"/>
+      <c r="Y9" s="131"/>
+      <c r="Z9" s="131"/>
+      <c r="AA9" s="131"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
@@ -8642,15 +8601,15 @@
         <v>0</v>
       </c>
       <c r="L10" s="75">
-        <v>4000</v>
+        <v>400000</v>
       </c>
       <c r="M10" s="26"/>
-      <c r="V10" s="140"/>
-      <c r="W10" s="140"/>
-      <c r="X10" s="140"/>
-      <c r="Y10" s="140"/>
-      <c r="Z10" s="140"/>
-      <c r="AA10" s="140"/>
+      <c r="V10" s="131"/>
+      <c r="W10" s="131"/>
+      <c r="X10" s="131"/>
+      <c r="Y10" s="131"/>
+      <c r="Z10" s="131"/>
+      <c r="AA10" s="131"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
@@ -8683,14 +8642,14 @@
         <v>0</v>
       </c>
       <c r="L11" s="75">
-        <v>4000</v>
-      </c>
-      <c r="V11" s="140"/>
-      <c r="W11" s="140"/>
-      <c r="X11" s="140"/>
-      <c r="Y11" s="140"/>
-      <c r="Z11" s="140"/>
-      <c r="AA11" s="140"/>
+        <v>400000</v>
+      </c>
+      <c r="V11" s="131"/>
+      <c r="W11" s="131"/>
+      <c r="X11" s="131"/>
+      <c r="Y11" s="131"/>
+      <c r="Z11" s="131"/>
+      <c r="AA11" s="131"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
@@ -8705,51 +8664,51 @@
       <c r="J12" s="49"/>
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
-      <c r="V12" s="140"/>
-      <c r="W12" s="140"/>
-      <c r="X12" s="140"/>
-      <c r="Y12" s="140"/>
-      <c r="Z12" s="140"/>
-      <c r="AA12" s="140"/>
+      <c r="V12" s="131"/>
+      <c r="W12" s="131"/>
+      <c r="X12" s="131"/>
+      <c r="Y12" s="131"/>
+      <c r="Z12" s="131"/>
+      <c r="AA12" s="131"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="Q13" s="49"/>
-      <c r="V13" s="140"/>
-      <c r="W13" s="140"/>
-      <c r="X13" s="140"/>
-      <c r="Y13" s="140"/>
-      <c r="Z13" s="140"/>
-      <c r="AA13" s="140"/>
+      <c r="V13" s="131"/>
+      <c r="W13" s="131"/>
+      <c r="X13" s="131"/>
+      <c r="Y13" s="131"/>
+      <c r="Z13" s="131"/>
+      <c r="AA13" s="131"/>
     </row>
     <row r="14" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="122" t="s">
+      <c r="A14" s="120" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="123"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="123"/>
-      <c r="H14" s="123"/>
-      <c r="I14" s="123"/>
-      <c r="J14" s="123"/>
-      <c r="K14" s="123"/>
-      <c r="L14" s="123"/>
-      <c r="M14" s="123"/>
-      <c r="N14" s="123"/>
-      <c r="O14" s="123"/>
-      <c r="P14" s="123"/>
+      <c r="B14" s="121"/>
+      <c r="C14" s="121"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="121"/>
+      <c r="H14" s="121"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="121"/>
+      <c r="K14" s="121"/>
+      <c r="L14" s="121"/>
+      <c r="M14" s="121"/>
+      <c r="N14" s="121"/>
+      <c r="O14" s="121"/>
+      <c r="P14" s="121"/>
       <c r="Q14" s="49"/>
       <c r="R14" s="35"/>
       <c r="S14" s="35"/>
       <c r="T14" s="35"/>
-      <c r="V14" s="140"/>
-      <c r="W14" s="140"/>
-      <c r="X14" s="140"/>
-      <c r="Y14" s="140"/>
-      <c r="Z14" s="140"/>
-      <c r="AA14" s="140"/>
+      <c r="V14" s="131"/>
+      <c r="W14" s="131"/>
+      <c r="X14" s="131"/>
+      <c r="Y14" s="131"/>
+      <c r="Z14" s="131"/>
+      <c r="AA14" s="131"/>
     </row>
     <row r="15" spans="1:27" s="35" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
@@ -8767,24 +8726,24 @@
       <c r="E15" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="130" t="s">
+      <c r="F15" s="142" t="s">
         <v>83</v>
       </c>
-      <c r="G15" s="130"/>
-      <c r="H15" s="130"/>
+      <c r="G15" s="142"/>
+      <c r="H15" s="142"/>
       <c r="I15" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="J15" s="137" t="s">
+      <c r="J15" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="138"/>
-      <c r="L15" s="139"/>
-      <c r="M15" s="136" t="s">
+      <c r="K15" s="148"/>
+      <c r="L15" s="149"/>
+      <c r="M15" s="146" t="s">
         <v>77</v>
       </c>
-      <c r="N15" s="136"/>
-      <c r="O15" s="136"/>
+      <c r="N15" s="146"/>
+      <c r="O15" s="146"/>
       <c r="P15" s="36" t="s">
         <v>79</v>
       </c>
@@ -8835,20 +8794,20 @@
       <c r="T17" s="38"/>
     </row>
     <row r="18" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="116" t="s">
+      <c r="A18" s="118" t="s">
         <v>151</v>
       </c>
-      <c r="B18" s="116"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="116"/>
-      <c r="F18" s="116"/>
-      <c r="G18" s="116"/>
-      <c r="H18" s="116"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="116"/>
-      <c r="K18" s="116"/>
-      <c r="L18" s="116"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="118"/>
+      <c r="L18" s="118"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
@@ -8866,16 +8825,16 @@
       <c r="E19" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="81" t="s">
+      <c r="F19" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="87" t="s">
+      <c r="G19" s="77"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="98" t="s">
         <v>160</v>
       </c>
-      <c r="J19" s="115"/>
-      <c r="K19" s="88"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="99"/>
       <c r="L19" s="33" t="s">
         <v>161</v>
       </c>
@@ -8947,6 +8906,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="J15:L15"/>
     <mergeCell ref="V2:AA14"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="R3:S3"/>
@@ -8958,15 +8926,6 @@
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="N8:R8"/>
     <mergeCell ref="A7:R7"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="J15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8989,21 +8948,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="F1" s="82" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="F1" s="108" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="I1" s="82" t="s">
+      <c r="G1" s="110"/>
+      <c r="I1" s="108" t="s">
         <v>240</v>
       </c>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="84"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="110"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
@@ -9021,12 +8980,12 @@
       <c r="G2" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="140" t="s">
+      <c r="I2" s="131" t="s">
         <v>239</v>
       </c>
-      <c r="J2" s="140"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="61"/>
@@ -9038,10 +8997,10 @@
       <c r="G3" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="I3" s="140"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="131"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="61"/>
@@ -9053,10 +9012,10 @@
       <c r="G4" s="62" t="s">
         <v>167</v>
       </c>
-      <c r="I4" s="140"/>
-      <c r="J4" s="140"/>
-      <c r="K4" s="140"/>
-      <c r="L4" s="140"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="61"/>
@@ -9068,10 +9027,10 @@
       <c r="G5" s="62" t="s">
         <v>170</v>
       </c>
-      <c r="I5" s="140"/>
-      <c r="J5" s="140"/>
-      <c r="K5" s="140"/>
-      <c r="L5" s="140"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="131"/>
+      <c r="L5" s="131"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="61"/>
@@ -9083,10 +9042,10 @@
       <c r="G6" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="I6" s="140"/>
-      <c r="J6" s="140"/>
-      <c r="K6" s="140"/>
-      <c r="L6" s="140"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="131"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="61"/>

</xml_diff>